<commit_message>
read the docs tidy up
</commit_message>
<xml_diff>
--- a/docs/Examples/Example1c_HORIBA_Calibration/Medium_Diads.xlsx
+++ b/docs/Examples/Example1c_HORIBA_Calibration/Medium_Diads.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AM12"/>
+  <dimension ref="A1:AM14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -633,41 +633,41 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>10mol_FID_R1</t>
+          <t>10mol_FID_R1_CRR_DiadFit</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>102.8297816623619</v>
+        <v>102.8377638935765</v>
       </c>
       <c r="C2" t="n">
-        <v>0.05023944421230666</v>
+        <v>0.04959893527708257</v>
       </c>
       <c r="D2" t="n">
-        <v>1285.53461603697</v>
+        <v>1285.527122961094</v>
       </c>
       <c r="E2" t="n">
-        <v>0.01925590143592911</v>
+        <v>0.01178480629337182</v>
       </c>
       <c r="F2" t="n">
-        <v>5704.425729670282</v>
+        <v>5619.914244325592</v>
       </c>
       <c r="G2" t="n">
-        <v>1285.53476604447</v>
+        <v>1285.527272968595</v>
       </c>
       <c r="H2" t="n">
-        <v>17339.91092277277</v>
+        <v>16313.78711437915</v>
       </c>
       <c r="I2" t="n">
-        <v>1.101368378777843</v>
+        <v>1.108288778719526</v>
       </c>
       <c r="J2" t="n">
-        <v>63.86407958999529</v>
+        <v>34.96559525188485</v>
       </c>
       <c r="K2" t="n">
-        <v>0.7139833430808202</v>
+        <v>0.5845425140259041</v>
       </c>
       <c r="L2" t="n">
-        <v>2.202736757555686</v>
+        <v>2.216577557439051</v>
       </c>
       <c r="M2" t="inlineStr">
         <is>
@@ -675,34 +675,34 @@
         </is>
       </c>
       <c r="N2" t="n">
-        <v>1388.364597709332</v>
+        <v>1388.365086864671</v>
       </c>
       <c r="O2" t="n">
-        <v>0.04640271559565513</v>
+        <v>0.04817855042700984</v>
       </c>
       <c r="P2" t="n">
-        <v>12770.36188984475</v>
+        <v>12748.39514501475</v>
       </c>
       <c r="Q2" t="n">
-        <v>1388.364547706832</v>
+        <v>1388.365036862171</v>
       </c>
       <c r="R2" t="n">
-        <v>27683.78963159475</v>
+        <v>27687.72380399519</v>
       </c>
       <c r="S2" t="n">
-        <v>0.6989648626925712</v>
+        <v>0.7003508821376203</v>
       </c>
       <c r="T2" t="n">
         <v>0</v>
       </c>
       <c r="U2" t="n">
-        <v>61.01375329336911</v>
+        <v>63.31064651813553</v>
       </c>
       <c r="V2" t="n">
-        <v>0.9731846226408309</v>
+        <v>0.9729330494900215</v>
       </c>
       <c r="W2" t="n">
-        <v>1.397929725385142</v>
+        <v>1.400701764275241</v>
       </c>
       <c r="X2" t="inlineStr">
         <is>
@@ -710,22 +710,22 @@
         </is>
       </c>
       <c r="Y2" t="n">
-        <v>1265.47569312381</v>
+        <v>1265.419626765947</v>
       </c>
       <c r="Z2" t="n">
-        <v>4411.341887327028</v>
+        <v>3360.928850803885</v>
       </c>
       <c r="AA2" t="n">
-        <v>3.285138212487888</v>
+        <v>3.308806523581385</v>
       </c>
       <c r="AB2" t="n">
-        <v>1409.823477912848</v>
+        <v>1409.825158078468</v>
       </c>
       <c r="AC2" t="n">
-        <v>2763.306030075118</v>
+        <v>2758.629638650139</v>
       </c>
       <c r="AD2" t="n">
-        <v>1.211140673630662</v>
+        <v>1.205365528947979</v>
       </c>
       <c r="AE2" t="inlineStr"/>
       <c r="AF2" t="inlineStr"/>
@@ -740,41 +740,41 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>10mol_FID_R1_FIN</t>
+          <t>10mol_FID_R1_FIN_CRR_DiadFit</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>102.8744566913222</v>
+        <v>102.8816922248814</v>
       </c>
       <c r="C3" t="n">
-        <v>0.02125424208406619</v>
+        <v>0.01778537260599995</v>
       </c>
       <c r="D3" t="n">
-        <v>1285.52810397633</v>
+        <v>1285.522277125933</v>
       </c>
       <c r="E3" t="n">
-        <v>0.01440244853852916</v>
+        <v>0.008969950063236261</v>
       </c>
       <c r="F3" t="n">
-        <v>5550.470276452032</v>
+        <v>5489.14332544442</v>
       </c>
       <c r="G3" t="n">
-        <v>1285.52825398383</v>
+        <v>1285.522327128433</v>
       </c>
       <c r="H3" t="n">
-        <v>15962.1583541836</v>
+        <v>15308.30541612356</v>
       </c>
       <c r="I3" t="n">
-        <v>1.088765242043368</v>
+        <v>1.094293396827522</v>
       </c>
       <c r="J3" t="n">
-        <v>46.61114281281026</v>
+        <v>26.17719556965784</v>
       </c>
       <c r="K3" t="n">
-        <v>0.60596435567417</v>
+        <v>0.512838040156941</v>
       </c>
       <c r="L3" t="n">
-        <v>2.177530484086736</v>
+        <v>2.188586793655045</v>
       </c>
       <c r="M3" t="inlineStr">
         <is>
@@ -782,34 +782,34 @@
         </is>
       </c>
       <c r="N3" t="n">
-        <v>1388.402760677653</v>
+        <v>1388.404069355814</v>
       </c>
       <c r="O3" t="n">
-        <v>0.01563049208000533</v>
+        <v>0.01535771710239843</v>
       </c>
       <c r="P3" t="n">
-        <v>11083.81878449055</v>
+        <v>11048.29180216056</v>
       </c>
       <c r="Q3" t="n">
-        <v>1388.402710675153</v>
+        <v>1388.404019353314</v>
       </c>
       <c r="R3" t="n">
-        <v>24886.17126450297</v>
+        <v>24828.20620298378</v>
       </c>
       <c r="S3" t="n">
-        <v>0.8037740373693865</v>
+        <v>0.8067679687518829</v>
       </c>
       <c r="T3" t="n">
         <v>0</v>
       </c>
       <c r="U3" t="n">
-        <v>37.58166595637027</v>
+        <v>36.33241671432218</v>
       </c>
       <c r="V3" t="n">
-        <v>0.7384306521014966</v>
+        <v>0.7316902044152861</v>
       </c>
       <c r="W3" t="n">
-        <v>1.607548074738773</v>
+        <v>1.613535937503766</v>
       </c>
       <c r="X3" t="inlineStr">
         <is>
@@ -817,22 +817,22 @@
         </is>
       </c>
       <c r="Y3" t="n">
-        <v>1265.092041520787</v>
+        <v>1265.310632515282</v>
       </c>
       <c r="Z3" t="n">
-        <v>3782.384548963773</v>
+        <v>2592.92571403285</v>
       </c>
       <c r="AA3" t="n">
-        <v>3.245753946556341</v>
+        <v>2.196131621968241</v>
       </c>
       <c r="AB3" t="n">
-        <v>1409.862546535232</v>
+        <v>1409.868565185193</v>
       </c>
       <c r="AC3" t="n">
-        <v>2661.9678414512</v>
+        <v>2605.88697117128</v>
       </c>
       <c r="AD3" t="n">
-        <v>1.208986130677894</v>
+        <v>1.182390379913012</v>
       </c>
       <c r="AE3" t="inlineStr"/>
       <c r="AF3" t="inlineStr"/>
@@ -847,41 +847,41 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>10mol_FID_R2</t>
+          <t>10mol_FID_R2_CRR_DiadFit</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>102.8542496341463</v>
+        <v>102.8642383184858</v>
       </c>
       <c r="C4" t="n">
-        <v>0.02145524117464217</v>
+        <v>0.01668901167673268</v>
       </c>
       <c r="D4" t="n">
-        <v>1285.630144934463</v>
+        <v>1285.621099291102</v>
       </c>
       <c r="E4" t="n">
-        <v>0.01730306371605134</v>
+        <v>0.01123530631824392</v>
       </c>
       <c r="F4" t="n">
-        <v>4908.770508369234</v>
+        <v>4828.888698490833</v>
       </c>
       <c r="G4" t="n">
-        <v>1285.630194936963</v>
+        <v>1285.621149293602</v>
       </c>
       <c r="H4" t="n">
-        <v>14006.84259363314</v>
+        <v>13405.09207817295</v>
       </c>
       <c r="I4" t="n">
-        <v>1.045212850667877</v>
+        <v>1.057224085658327</v>
       </c>
       <c r="J4" t="n">
-        <v>43.52891122925847</v>
+        <v>27.09294568684872</v>
       </c>
       <c r="K4" t="n">
-        <v>0.6865959844213715</v>
+        <v>0.5885014511733845</v>
       </c>
       <c r="L4" t="n">
-        <v>2.090425701335754</v>
+        <v>2.114448171316654</v>
       </c>
       <c r="M4" t="inlineStr">
         <is>
@@ -889,34 +889,34 @@
         </is>
       </c>
       <c r="N4" t="n">
-        <v>1388.48449457361</v>
+        <v>1388.485437614588</v>
       </c>
       <c r="O4" t="n">
-        <v>0.01268587245325793</v>
+        <v>0.01234062407989758</v>
       </c>
       <c r="P4" t="n">
-        <v>8714.908536047416</v>
+        <v>8704.216587182647</v>
       </c>
       <c r="Q4" t="n">
-        <v>1388.48444457111</v>
+        <v>1388.485387612088</v>
       </c>
       <c r="R4" t="n">
-        <v>21840.68418931988</v>
+        <v>21814.18747834233</v>
       </c>
       <c r="S4" t="n">
-        <v>0.9054786513560038</v>
+        <v>0.9074702277706672</v>
       </c>
       <c r="T4" t="n">
         <v>0</v>
       </c>
       <c r="U4" t="n">
-        <v>38.22815526277259</v>
+        <v>37.36224587794332</v>
       </c>
       <c r="V4" t="n">
-        <v>0.7165292787796714</v>
+        <v>0.7113018170177456</v>
       </c>
       <c r="W4" t="n">
-        <v>1.810957302712008</v>
+        <v>1.814940455541334</v>
       </c>
       <c r="X4" t="inlineStr">
         <is>
@@ -924,22 +924,22 @@
         </is>
       </c>
       <c r="Y4" t="n">
-        <v>1265.213010308015</v>
+        <v>1265.259057138157</v>
       </c>
       <c r="Z4" t="n">
-        <v>3109.393528420597</v>
+        <v>1977.860323983438</v>
       </c>
       <c r="AA4" t="n">
-        <v>3.108434855517081</v>
+        <v>1.914679705677203</v>
       </c>
       <c r="AB4" t="n">
-        <v>1409.80645799793</v>
+        <v>1409.814392167124</v>
       </c>
       <c r="AC4" t="n">
-        <v>2224.474217579083</v>
+        <v>2202.140146083395</v>
       </c>
       <c r="AD4" t="n">
-        <v>1.178480902361383</v>
+        <v>1.159513756611419</v>
       </c>
       <c r="AE4" t="inlineStr"/>
       <c r="AF4" t="inlineStr"/>
@@ -954,41 +954,41 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>10mol_FID_R2_FIN</t>
+          <t>10mol_FID_R2_FIN_CRR_DiadFit</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>102.8959598024971</v>
+        <v>102.9067318552393</v>
       </c>
       <c r="C5" t="n">
-        <v>0.02107098764556824</v>
+        <v>0.01466523054853881</v>
       </c>
       <c r="D5" t="n">
-        <v>1285.5785074694</v>
+        <v>1285.569165309289</v>
       </c>
       <c r="E5" t="n">
-        <v>0.01838614784221907</v>
+        <v>0.01058770117482047</v>
       </c>
       <c r="F5" t="n">
-        <v>5218.873863571061</v>
+        <v>5129.330337292101</v>
       </c>
       <c r="G5" t="n">
-        <v>1285.578657476901</v>
+        <v>1285.569215311789</v>
       </c>
       <c r="H5" t="n">
-        <v>15691.43690647814</v>
+        <v>14790.86211887556</v>
       </c>
       <c r="I5" t="n">
-        <v>1.108906863448731</v>
+        <v>1.118502795955241</v>
       </c>
       <c r="J5" t="n">
-        <v>57.32403151773683</v>
+        <v>31.27747078052134</v>
       </c>
       <c r="K5" t="n">
-        <v>0.6708984188901168</v>
+        <v>0.5428415722616939</v>
       </c>
       <c r="L5" t="n">
-        <v>2.217813726897462</v>
+        <v>2.237005591910481</v>
       </c>
       <c r="M5" t="inlineStr">
         <is>
@@ -996,34 +996,34 @@
         </is>
       </c>
       <c r="N5" t="n">
-        <v>1388.474667281898</v>
+        <v>1388.475997169528</v>
       </c>
       <c r="O5" t="n">
-        <v>0.01029252582623684</v>
+        <v>0.01014739231894093</v>
       </c>
       <c r="P5" t="n">
-        <v>9340.739847605499</v>
+        <v>9324.939272200729</v>
       </c>
       <c r="Q5" t="n">
-        <v>1388.474617279398</v>
+        <v>1388.475947167028</v>
       </c>
       <c r="R5" t="n">
-        <v>22941.53671449018</v>
+        <v>22897.05863248581</v>
       </c>
       <c r="S5" t="n">
-        <v>0.9028830723118442</v>
+        <v>0.9055510637620972</v>
       </c>
       <c r="T5" t="n">
         <v>0</v>
       </c>
       <c r="U5" t="n">
-        <v>33.09869417900052</v>
+        <v>33.23993301473777</v>
       </c>
       <c r="V5" t="n">
-        <v>0.6749848093667785</v>
+        <v>0.667202744244098</v>
       </c>
       <c r="W5" t="n">
-        <v>1.805766144623688</v>
+        <v>1.811102127524194</v>
       </c>
       <c r="X5" t="inlineStr">
         <is>
@@ -1031,22 +1031,22 @@
         </is>
       </c>
       <c r="Y5" t="n">
-        <v>1265.181673429521</v>
+        <v>1265.263150243659</v>
       </c>
       <c r="Z5" t="n">
-        <v>3887.894723247436</v>
+        <v>2487.426048761728</v>
       </c>
       <c r="AA5" t="n">
-        <v>3.30373937089081</v>
+        <v>2.506182747792088</v>
       </c>
       <c r="AB5" t="n">
-        <v>1409.840931248001</v>
+        <v>1409.84380198324</v>
       </c>
       <c r="AC5" t="n">
-        <v>2715.078113657602</v>
+        <v>2701.449428341389</v>
       </c>
       <c r="AD5" t="n">
-        <v>1.245478188824122</v>
+        <v>1.236657105020613</v>
       </c>
       <c r="AE5" t="inlineStr"/>
       <c r="AF5" t="inlineStr"/>
@@ -1061,41 +1061,41 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>10mol_FID_R3</t>
+          <t>10mol_FID_R3_CRR_DiadFit</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>102.9362534979073</v>
+        <v>102.9586732225598</v>
       </c>
       <c r="C6" t="n">
-        <v>0.05292771991495908</v>
+        <v>0.03388632283157626</v>
       </c>
       <c r="D6" t="n">
-        <v>1285.55058686565</v>
+        <v>1285.529762173011</v>
       </c>
       <c r="E6" t="n">
-        <v>0.04917238991857218</v>
+        <v>0.02833614406438176</v>
       </c>
       <c r="F6" t="n">
-        <v>2731.390502113231</v>
+        <v>2622.783493579976</v>
       </c>
       <c r="G6" t="n">
-        <v>1285.55073687315</v>
+        <v>1285.529812175512</v>
       </c>
       <c r="H6" t="n">
-        <v>8297.013952210233</v>
+        <v>7104.212376365639</v>
       </c>
       <c r="I6" t="n">
-        <v>1.064870650181074</v>
+        <v>1.086294248379287</v>
       </c>
       <c r="J6" t="n">
-        <v>62.37235133014627</v>
+        <v>34.07388422500614</v>
       </c>
       <c r="K6" t="n">
-        <v>0.7916668452220912</v>
+        <v>0.4537801546949451</v>
       </c>
       <c r="L6" t="n">
-        <v>2.129741300362149</v>
+        <v>2.172588496758574</v>
       </c>
       <c r="M6" t="inlineStr">
         <is>
@@ -1103,34 +1103,34 @@
         </is>
       </c>
       <c r="N6" t="n">
-        <v>1388.487040373558</v>
+        <v>1388.488535400571</v>
       </c>
       <c r="O6" t="n">
-        <v>0.01958110326545104</v>
+        <v>0.01858348230575768</v>
       </c>
       <c r="P6" t="n">
-        <v>5018.921569443069</v>
+        <v>5008.289215736333</v>
       </c>
       <c r="Q6" t="n">
-        <v>1388.486990371058</v>
+        <v>1388.488485398071</v>
       </c>
       <c r="R6" t="n">
-        <v>11956.63368467653</v>
+        <v>11935.96375800689</v>
       </c>
       <c r="S6" t="n">
-        <v>0.8631858595140782</v>
+        <v>0.8662430099209146</v>
       </c>
       <c r="T6" t="n">
         <v>0</v>
       </c>
       <c r="U6" t="n">
-        <v>27.42228488978235</v>
+        <v>26.65920975537803</v>
       </c>
       <c r="V6" t="n">
-        <v>0.7098638556235178</v>
+        <v>0.7023269672618326</v>
       </c>
       <c r="W6" t="n">
-        <v>1.726371719028156</v>
+        <v>1.732486019841829</v>
       </c>
       <c r="X6" t="inlineStr">
         <is>
@@ -1138,22 +1138,22 @@
         </is>
       </c>
       <c r="Y6" t="n">
-        <v>1264.687545215333</v>
+        <v>1264.928859119508</v>
       </c>
       <c r="Z6" t="n">
-        <v>2416.460636952165</v>
+        <v>922.3762580309841</v>
       </c>
       <c r="AA6" t="n">
-        <v>3.175036234928037</v>
+        <v>0.3881986783096811</v>
       </c>
       <c r="AB6" t="n">
-        <v>1409.77403290828</v>
+        <v>1409.774043463867</v>
       </c>
       <c r="AC6" t="n">
-        <v>1377.124352450057</v>
+        <v>1375.781096561233</v>
       </c>
       <c r="AD6" t="n">
-        <v>1.363842734041126</v>
+        <v>1.363662595136703</v>
       </c>
       <c r="AE6" t="inlineStr"/>
       <c r="AF6" t="inlineStr"/>
@@ -1168,41 +1168,41 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>10mol_FID_R3_FIN</t>
+          <t>10mol_FID_R3_FIN_CRR_DiadFit</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>102.8818505540471</v>
+        <v>102.8984064222309</v>
       </c>
       <c r="C7" t="n">
-        <v>0.03899765602352875</v>
+        <v>0.02441482666403032</v>
       </c>
       <c r="D7" t="n">
-        <v>1285.552477827614</v>
+        <v>1285.53544077659</v>
       </c>
       <c r="E7" t="n">
-        <v>0.03567405823195143</v>
+        <v>0.01854393823185304</v>
       </c>
       <c r="F7" t="n">
-        <v>3578.279407580177</v>
+        <v>3468.31711470991</v>
       </c>
       <c r="G7" t="n">
-        <v>1285.552627835115</v>
+        <v>1285.53549077909</v>
       </c>
       <c r="H7" t="n">
-        <v>10822.18219539805</v>
+        <v>9691.442455642982</v>
       </c>
       <c r="I7" t="n">
-        <v>1.071875904316202</v>
+        <v>1.089636498475765</v>
       </c>
       <c r="J7" t="n">
-        <v>63.6099645101126</v>
+        <v>31.14639016302728</v>
       </c>
       <c r="K7" t="n">
-        <v>0.7663122255625729</v>
+        <v>0.5282068920168109</v>
       </c>
       <c r="L7" t="n">
-        <v>2.143751808632404</v>
+        <v>2.179272996951529</v>
       </c>
       <c r="M7" t="inlineStr">
         <is>
@@ -1210,34 +1210,34 @@
         </is>
       </c>
       <c r="N7" t="n">
-        <v>1388.434528391662</v>
+        <v>1388.433947203821</v>
       </c>
       <c r="O7" t="n">
-        <v>0.01575368987230632</v>
+        <v>0.0158809985796821</v>
       </c>
       <c r="P7" t="n">
-        <v>6742.498063020919</v>
+        <v>6750.770434650058</v>
       </c>
       <c r="Q7" t="n">
-        <v>1388.434478389162</v>
+        <v>1388.433897201321</v>
       </c>
       <c r="R7" t="n">
-        <v>15400.83761935538</v>
+        <v>15417.95830552551</v>
       </c>
       <c r="S7" t="n">
-        <v>0.8267709105215055</v>
+        <v>0.8255612495622753</v>
       </c>
       <c r="T7" t="n">
         <v>0</v>
       </c>
       <c r="U7" t="n">
-        <v>24.17588362899392</v>
+        <v>24.99665420683463</v>
       </c>
       <c r="V7" t="n">
-        <v>0.7122087024786896</v>
+        <v>0.7154405126191407</v>
       </c>
       <c r="W7" t="n">
-        <v>1.653541821043011</v>
+        <v>1.651122499124551</v>
       </c>
       <c r="X7" t="inlineStr">
         <is>
@@ -1245,22 +1245,22 @@
         </is>
       </c>
       <c r="Y7" t="n">
-        <v>1264.921042628507</v>
+        <v>1265.282065724438</v>
       </c>
       <c r="Z7" t="n">
-        <v>3101.57432016602</v>
+        <v>1404.221158830771</v>
       </c>
       <c r="AA7" t="n">
-        <v>3.19171943121368</v>
+        <v>1.720606377409798</v>
       </c>
       <c r="AB7" t="n">
-        <v>1409.950565237413</v>
+        <v>1409.948135490478</v>
       </c>
       <c r="AC7" t="n">
-        <v>1784.533176756058</v>
+        <v>1801.323232193023</v>
       </c>
       <c r="AD7" t="n">
-        <v>1.171015277681735</v>
+        <v>1.183144375516663</v>
       </c>
       <c r="AE7" t="inlineStr"/>
       <c r="AF7" t="inlineStr"/>
@@ -1275,41 +1275,41 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>10mol_FIE_R1</t>
+          <t>10mol_FIE_R1_CRR_DiadFit</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>102.8605567721506</v>
+        <v>102.8694876684419</v>
       </c>
       <c r="C8" t="n">
-        <v>0.06615677715558137</v>
+        <v>0.064059667821245</v>
       </c>
       <c r="D8" t="n">
-        <v>1285.472544493566</v>
+        <v>1285.462552484733</v>
       </c>
       <c r="E8" t="n">
-        <v>0.02563707772078044</v>
+        <v>0.01148120536646289</v>
       </c>
       <c r="F8" t="n">
-        <v>4677.893423069379</v>
+        <v>4580.616882483282</v>
       </c>
       <c r="G8" t="n">
-        <v>1285.472694501067</v>
+        <v>1285.462602487233</v>
       </c>
       <c r="H8" t="n">
-        <v>14067.02114573478</v>
+        <v>12785.13985608224</v>
       </c>
       <c r="I8" t="n">
-        <v>1.050558848567405</v>
+        <v>1.065018403047506</v>
       </c>
       <c r="J8" t="n">
-        <v>67.2568805811346</v>
+        <v>24.48543424709635</v>
       </c>
       <c r="K8" t="n">
-        <v>0.7997919568436864</v>
+        <v>0.5841908212725487</v>
       </c>
       <c r="L8" t="n">
-        <v>2.10111769713481</v>
+        <v>2.130036806095012</v>
       </c>
       <c r="M8" t="inlineStr">
         <is>
@@ -1317,34 +1317,34 @@
         </is>
       </c>
       <c r="N8" t="n">
-        <v>1388.333301275717</v>
+        <v>1388.332140158175</v>
       </c>
       <c r="O8" t="n">
-        <v>0.06098737090211314</v>
+        <v>0.06302240049935702</v>
       </c>
       <c r="P8" t="n">
-        <v>11467.97636576202</v>
+        <v>11549.85287937143</v>
       </c>
       <c r="Q8" t="n">
-        <v>1388.333251273217</v>
+        <v>1388.332090155675</v>
       </c>
       <c r="R8" t="n">
-        <v>22828.40767908173</v>
+        <v>22848.69853506233</v>
       </c>
       <c r="S8" t="n">
-        <v>0.636805578312812</v>
+        <v>0.6322885012030675</v>
       </c>
       <c r="T8" t="n">
         <v>0</v>
       </c>
       <c r="U8" t="n">
-        <v>55.18628608526273</v>
+        <v>54.91386576110205</v>
       </c>
       <c r="V8" t="n">
-        <v>0.9899295510191541</v>
+        <v>0.9917909471329743</v>
       </c>
       <c r="W8" t="n">
-        <v>1.273611156625624</v>
+        <v>1.264577002406135</v>
       </c>
       <c r="X8" t="inlineStr">
         <is>
@@ -1352,22 +1352,22 @@
         </is>
       </c>
       <c r="Y8" t="n">
-        <v>1265.384142021345</v>
+        <v>1265.404390404323</v>
       </c>
       <c r="Z8" t="n">
-        <v>4074.199858644757</v>
+        <v>2150.024988246679</v>
       </c>
       <c r="AA8" t="n">
-        <v>3.1288842655403</v>
+        <v>2.171810146594718</v>
       </c>
       <c r="AB8" t="n">
-        <v>1409.782332125115</v>
+        <v>1409.78944642188</v>
       </c>
       <c r="AC8" t="n">
-        <v>2551.920370441731</v>
+        <v>2502.131194891816</v>
       </c>
       <c r="AD8" t="n">
-        <v>1.389523746112236</v>
+        <v>1.352457767897226</v>
       </c>
       <c r="AE8" t="inlineStr"/>
       <c r="AF8" t="inlineStr"/>
@@ -1382,41 +1382,41 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>10mol_FIE_R1_FIN</t>
+          <t>10mol_FIE_R1_FIN_CRR_DiadFit</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>102.9075871396008</v>
+        <v>102.9152967249868</v>
       </c>
       <c r="C9" t="n">
-        <v>0.01790712259597834</v>
+        <v>0.01557727744969123</v>
       </c>
       <c r="D9" t="n">
-        <v>1285.746524183386</v>
+        <v>1285.738750619335</v>
       </c>
       <c r="E9" t="n">
-        <v>0.01415644581493901</v>
+        <v>0.01009876157176537</v>
       </c>
       <c r="F9" t="n">
-        <v>4950.344504350295</v>
+        <v>4859.132897018764</v>
       </c>
       <c r="G9" t="n">
-        <v>1285.746674190887</v>
+        <v>1285.738800621835</v>
       </c>
       <c r="H9" t="n">
-        <v>14084.99190382439</v>
+        <v>13530.01202404115</v>
       </c>
       <c r="I9" t="n">
-        <v>1.095846274884047</v>
+        <v>1.110128096113508</v>
       </c>
       <c r="J9" t="n">
-        <v>42.7729173104098</v>
+        <v>27.34134639354992</v>
       </c>
       <c r="K9" t="n">
-        <v>0.5628678348148524</v>
+        <v>0.4712418286724209</v>
       </c>
       <c r="L9" t="n">
-        <v>2.191692549768093</v>
+        <v>2.220256192227016</v>
       </c>
       <c r="M9" t="inlineStr">
         <is>
@@ -1424,34 +1424,34 @@
         </is>
       </c>
       <c r="N9" t="n">
-        <v>1388.654311332988</v>
+        <v>1388.654147349322</v>
       </c>
       <c r="O9" t="n">
-        <v>0.01096631576948675</v>
+        <v>0.01186029457734057</v>
       </c>
       <c r="P9" t="n">
-        <v>8463.14863754159</v>
+        <v>8466.407056169093</v>
       </c>
       <c r="Q9" t="n">
-        <v>1388.654261330488</v>
+        <v>1388.654097346822</v>
       </c>
       <c r="R9" t="n">
-        <v>21564.61301026278</v>
+        <v>21594.41638082521</v>
       </c>
       <c r="S9" t="n">
-        <v>0.9394391284618238</v>
+        <v>0.9392316178858893</v>
       </c>
       <c r="T9" t="n">
         <v>0</v>
       </c>
       <c r="U9" t="n">
-        <v>41.09670119583196</v>
+        <v>44.80042696790879</v>
       </c>
       <c r="V9" t="n">
-        <v>0.6678663406206226</v>
+        <v>0.6708440809428584</v>
       </c>
       <c r="W9" t="n">
-        <v>1.878878256923648</v>
+        <v>1.878463235771779</v>
       </c>
       <c r="X9" t="inlineStr">
         <is>
@@ -1459,22 +1459,22 @@
         </is>
       </c>
       <c r="Y9" t="n">
-        <v>1265.494093807688</v>
+        <v>1265.520889237378</v>
       </c>
       <c r="Z9" t="n">
-        <v>3422.245994565976</v>
+        <v>2291.365286474133</v>
       </c>
       <c r="AA9" t="n">
-        <v>3.242184545332766</v>
+        <v>2.211778413954403</v>
       </c>
       <c r="AB9" t="n">
-        <v>1410.007449654135</v>
+        <v>1410.003992410116</v>
       </c>
       <c r="AC9" t="n">
-        <v>2509.919471655886</v>
+        <v>2543.933232327188</v>
       </c>
       <c r="AD9" t="n">
-        <v>1.184274555531976</v>
+        <v>1.2013480838689</v>
       </c>
       <c r="AE9" t="inlineStr"/>
       <c r="AF9" t="inlineStr"/>
@@ -1489,41 +1489,41 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>10mol_FIE_R2</t>
+          <t>10mol_FIE_R2_CRR_DiadFit</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>102.9417809028055</v>
+        <v>102.9502299927717</v>
       </c>
       <c r="C10" t="n">
-        <v>0.02976619826299704</v>
+        <v>0.02773984986190029</v>
       </c>
       <c r="D10" t="n">
-        <v>1285.840776311663</v>
+        <v>1285.83382242556</v>
       </c>
       <c r="E10" t="n">
-        <v>0.02514939827587741</v>
+        <v>0.02250250415059966</v>
       </c>
       <c r="F10" t="n">
-        <v>1944.001420447771</v>
+        <v>1906.640135235176</v>
       </c>
       <c r="G10" t="n">
-        <v>1285.840926319163</v>
+        <v>1285.83397243306</v>
       </c>
       <c r="H10" t="n">
-        <v>5940.488760886211</v>
+        <v>5733.972110240618</v>
       </c>
       <c r="I10" t="n">
-        <v>1.144990736669777</v>
+        <v>1.165295645246683</v>
       </c>
       <c r="J10" t="n">
-        <v>26.98660741827854</v>
+        <v>23.33298352443612</v>
       </c>
       <c r="K10" t="n">
-        <v>0.6327408128086257</v>
+        <v>0.5480793557213668</v>
       </c>
       <c r="L10" t="n">
-        <v>2.289981473339553</v>
+        <v>2.330591290493365</v>
       </c>
       <c r="M10" t="inlineStr">
         <is>
@@ -1531,34 +1531,34 @@
         </is>
       </c>
       <c r="N10" t="n">
-        <v>1388.782757224469</v>
+        <v>1388.784252428332</v>
       </c>
       <c r="O10" t="n">
-        <v>0.01592276123646091</v>
+        <v>0.01622148505263975</v>
       </c>
       <c r="P10" t="n">
-        <v>3123.45622063233</v>
+        <v>3125.107688500002</v>
       </c>
       <c r="Q10" t="n">
-        <v>1388.782707221969</v>
+        <v>1388.784202425832</v>
       </c>
       <c r="R10" t="n">
-        <v>9440.178337860109</v>
+        <v>9372.520309767933</v>
       </c>
       <c r="S10" t="n">
-        <v>1.078390623964059</v>
+        <v>1.083305524840976</v>
       </c>
       <c r="T10" t="n">
         <v>0</v>
       </c>
       <c r="U10" t="n">
-        <v>24.59186767183375</v>
+        <v>26.10291939606723</v>
       </c>
       <c r="V10" t="n">
-        <v>0.7466143917854925</v>
+        <v>0.7175713155874466</v>
       </c>
       <c r="W10" t="n">
-        <v>2.156781247928119</v>
+        <v>2.166611049681952</v>
       </c>
       <c r="X10" t="inlineStr">
         <is>
@@ -1566,22 +1566,22 @@
         </is>
       </c>
       <c r="Y10" t="n">
-        <v>1265.887323519565</v>
+        <v>1265.721324302527</v>
       </c>
       <c r="Z10" t="n">
-        <v>1543.164030311852</v>
+        <v>1396.434520259221</v>
       </c>
       <c r="AA10" t="n">
-        <v>3.362664619137974</v>
+        <v>3.435087667284723</v>
       </c>
       <c r="AB10" t="n">
-        <v>1410.132890701866</v>
+        <v>1410.131169243524</v>
       </c>
       <c r="AC10" t="n">
-        <v>1172.427581590202</v>
+        <v>1198.938777129519</v>
       </c>
       <c r="AD10" t="n">
-        <v>1.402875011361988</v>
+        <v>1.429587408944799</v>
       </c>
       <c r="AE10" t="inlineStr"/>
       <c r="AF10" t="inlineStr"/>
@@ -1596,41 +1596,41 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>10mol_FIE_R2_FIN</t>
+          <t>10mol_FIE_R2_FIN_CRR_DiadFit</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>102.8553470750667</v>
+        <v>102.8710804536822</v>
       </c>
       <c r="C11" t="n">
-        <v>0.02659614146140798</v>
+        <v>0.02029492479995488</v>
       </c>
       <c r="D11" t="n">
-        <v>1285.634426259555</v>
+        <v>1285.619791299369</v>
       </c>
       <c r="E11" t="n">
-        <v>0.02006270648048184</v>
+        <v>0.009667602291843129</v>
       </c>
       <c r="F11" t="n">
-        <v>5649.995431707794</v>
+        <v>5494.013165135239</v>
       </c>
       <c r="G11" t="n">
-        <v>1285.634576267055</v>
+        <v>1285.619841301869</v>
       </c>
       <c r="H11" t="n">
-        <v>16532.03547445262</v>
+        <v>15270.17616114602</v>
       </c>
       <c r="I11" t="n">
-        <v>1.072123725286588</v>
+        <v>1.090723900593976</v>
       </c>
       <c r="J11" t="n">
-        <v>64.86290486943187</v>
+        <v>26.67041716807973</v>
       </c>
       <c r="K11" t="n">
-        <v>0.6867909901769325</v>
+        <v>0.5118352029319945</v>
       </c>
       <c r="L11" t="n">
-        <v>2.144247450573176</v>
+        <v>2.181447801187951</v>
       </c>
       <c r="M11" t="inlineStr">
         <is>
@@ -1638,34 +1638,34 @@
         </is>
       </c>
       <c r="N11" t="n">
-        <v>1388.489973344622</v>
+        <v>1388.490971758052</v>
       </c>
       <c r="O11" t="n">
-        <v>0.01745974081460709</v>
+        <v>0.01784436713819162</v>
       </c>
       <c r="P11" t="n">
-        <v>10339.55060636411</v>
+        <v>10322.98294214089</v>
       </c>
       <c r="Q11" t="n">
-        <v>1388.489923342122</v>
+        <v>1388.490921755552</v>
       </c>
       <c r="R11" t="n">
-        <v>24790.03981954176</v>
+        <v>24752.83299122084</v>
       </c>
       <c r="S11" t="n">
-        <v>0.8395706208591145</v>
+        <v>0.8416114507596639</v>
       </c>
       <c r="T11" t="n">
         <v>0</v>
       </c>
       <c r="U11" t="n">
-        <v>45.29613203027746</v>
+        <v>45.11399504771066</v>
       </c>
       <c r="V11" t="n">
-        <v>0.7900878483111995</v>
+        <v>0.7846927459199935</v>
       </c>
       <c r="W11" t="n">
-        <v>1.679141241718229</v>
+        <v>1.683222901519328</v>
       </c>
       <c r="X11" t="inlineStr">
         <is>
@@ -1673,22 +1673,22 @@
         </is>
       </c>
       <c r="Y11" t="n">
-        <v>1265.379426047034</v>
+        <v>1265.431256961675</v>
       </c>
       <c r="Z11" t="n">
-        <v>4325.922130958828</v>
+        <v>2133.174031573159</v>
       </c>
       <c r="AA11" t="n">
-        <v>3.18730448359353</v>
+        <v>1.745210418519898</v>
       </c>
       <c r="AB11" t="n">
-        <v>1409.905365656438</v>
+        <v>1409.908506107396</v>
       </c>
       <c r="AC11" t="n">
-        <v>2839.097625503804</v>
+        <v>2812.036657997331</v>
       </c>
       <c r="AD11" t="n">
-        <v>1.199262427954207</v>
+        <v>1.185923928141579</v>
       </c>
       <c r="AE11" t="inlineStr"/>
       <c r="AF11" t="inlineStr"/>
@@ -1703,41 +1703,41 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>10mol_FIE_R3_FIN</t>
+          <t>10mol_FIE_R3_CRR_DiadFit</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>102.8630519623539</v>
+        <v>102.8055562153388</v>
       </c>
       <c r="C12" t="n">
-        <v>0.02495548329592735</v>
+        <v>0.1199538242310884</v>
       </c>
       <c r="D12" t="n">
-        <v>1285.707790853106</v>
+        <v>1285.966629557231</v>
       </c>
       <c r="E12" t="n">
-        <v>0.01911671263382405</v>
+        <v>0.1088151117474008</v>
       </c>
       <c r="F12" t="n">
-        <v>3874.7172050717</v>
+        <v>990.9389532829739</v>
       </c>
       <c r="G12" t="n">
-        <v>1285.707940860607</v>
+        <v>1285.966779564731</v>
       </c>
       <c r="H12" t="n">
-        <v>11695.24350765689</v>
+        <v>2847.311005631103</v>
       </c>
       <c r="I12" t="n">
-        <v>1.129259275061858</v>
+        <v>1.070946645178667</v>
       </c>
       <c r="J12" t="n">
-        <v>45.8357151667217</v>
+        <v>59.07913569912772</v>
       </c>
       <c r="K12" t="n">
-        <v>0.6363737299197317</v>
+        <v>0.6456765686679995</v>
       </c>
       <c r="L12" t="n">
-        <v>2.258518550123715</v>
+        <v>2.141893290357334</v>
       </c>
       <c r="M12" t="inlineStr">
         <is>
@@ -1745,34 +1745,34 @@
         </is>
       </c>
       <c r="N12" t="n">
-        <v>1388.571042825461</v>
+        <v>1388.77238578257</v>
       </c>
       <c r="O12" t="n">
-        <v>0.01604142900770069</v>
+        <v>0.05047961373726567</v>
       </c>
       <c r="P12" t="n">
-        <v>6558.270965357585</v>
+        <v>1546.376832783989</v>
       </c>
       <c r="Q12" t="n">
-        <v>1388.570992822961</v>
+        <v>1388.77233578007</v>
       </c>
       <c r="R12" t="n">
-        <v>17479.64183410967</v>
+        <v>5598.235544243918</v>
       </c>
       <c r="S12" t="n">
-        <v>0.9311224984755757</v>
+        <v>1.152853579350377</v>
       </c>
       <c r="T12" t="n">
         <v>0</v>
       </c>
       <c r="U12" t="n">
-        <v>37.64113535494664</v>
+        <v>28.15121834854718</v>
       </c>
       <c r="V12" t="n">
-        <v>0.7956868654577967</v>
+        <v>0.9999999999846203</v>
       </c>
       <c r="W12" t="n">
-        <v>1.862244996951151</v>
+        <v>2.305707158700754</v>
       </c>
       <c r="X12" t="inlineStr">
         <is>
@@ -1780,22 +1780,22 @@
         </is>
       </c>
       <c r="Y12" t="n">
-        <v>1265.306655298167</v>
+        <v>1265.017000102856</v>
       </c>
       <c r="Z12" t="n">
-        <v>3179.701001582481</v>
+        <v>938.8168766896518</v>
       </c>
       <c r="AA12" t="n">
-        <v>3.348070290848418</v>
+        <v>3.029596737184817</v>
       </c>
       <c r="AB12" t="n">
-        <v>1409.960262053374</v>
+        <v>1410.147167684385</v>
       </c>
       <c r="AC12" t="n">
-        <v>2236.302481339537</v>
+        <v>601.0069468703052</v>
       </c>
       <c r="AD12" t="n">
-        <v>1.303648770344346</v>
+        <v>1.609046155398191</v>
       </c>
       <c r="AE12" t="inlineStr"/>
       <c r="AF12" t="inlineStr"/>
@@ -1807,6 +1807,220 @@
       <c r="AL12" t="inlineStr"/>
       <c r="AM12" t="inlineStr"/>
     </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>10mol_FIE_R3_FIN_CRR_DiadFit</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>102.8733362612959</v>
+      </c>
+      <c r="C13" t="n">
+        <v>0.02102195037842777</v>
+      </c>
+      <c r="D13" t="n">
+        <v>1285.697402702577</v>
+      </c>
+      <c r="E13" t="n">
+        <v>0.01238677559362235</v>
+      </c>
+      <c r="F13" t="n">
+        <v>3790.954889438735</v>
+      </c>
+      <c r="G13" t="n">
+        <v>1285.697552710077</v>
+      </c>
+      <c r="H13" t="n">
+        <v>11050.60299877951</v>
+      </c>
+      <c r="I13" t="n">
+        <v>1.145042811691213</v>
+      </c>
+      <c r="J13" t="n">
+        <v>27.44051118547585</v>
+      </c>
+      <c r="K13" t="n">
+        <v>0.5122997847891189</v>
+      </c>
+      <c r="L13" t="n">
+        <v>2.290085623382425</v>
+      </c>
+      <c r="M13" t="inlineStr">
+        <is>
+          <t>Flagged Warnings:</t>
+        </is>
+      </c>
+      <c r="N13" t="n">
+        <v>1388.570938973873</v>
+      </c>
+      <c r="O13" t="n">
+        <v>0.01698499891393348</v>
+      </c>
+      <c r="P13" t="n">
+        <v>6559.353842181924</v>
+      </c>
+      <c r="Q13" t="n">
+        <v>1388.570888971373</v>
+      </c>
+      <c r="R13" t="n">
+        <v>17486.78458467075</v>
+      </c>
+      <c r="S13" t="n">
+        <v>0.9309953957347812</v>
+      </c>
+      <c r="T13" t="n">
+        <v>0</v>
+      </c>
+      <c r="U13" t="n">
+        <v>39.65755746251234</v>
+      </c>
+      <c r="V13" t="n">
+        <v>0.7965454650936415</v>
+      </c>
+      <c r="W13" t="n">
+        <v>1.861990791469562</v>
+      </c>
+      <c r="X13" t="inlineStr">
+        <is>
+          <t>Flagged Warnings:</t>
+        </is>
+      </c>
+      <c r="Y13" t="n">
+        <v>1265.334899975337</v>
+      </c>
+      <c r="Z13" t="n">
+        <v>2506.779841938958</v>
+      </c>
+      <c r="AA13" t="n">
+        <v>3.400539436517786</v>
+      </c>
+      <c r="AB13" t="n">
+        <v>1409.966725362087</v>
+      </c>
+      <c r="AC13" t="n">
+        <v>2217.503359961111</v>
+      </c>
+      <c r="AD13" t="n">
+        <v>1.282871070503112</v>
+      </c>
+      <c r="AE13" t="inlineStr"/>
+      <c r="AF13" t="inlineStr"/>
+      <c r="AG13" t="inlineStr"/>
+      <c r="AH13" t="inlineStr"/>
+      <c r="AI13" t="inlineStr"/>
+      <c r="AJ13" t="inlineStr"/>
+      <c r="AK13" t="inlineStr"/>
+      <c r="AL13" t="inlineStr"/>
+      <c r="AM13" t="inlineStr"/>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>1mol_FIB_R1_CRR_DiadFit</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>102.7452797308244</v>
+      </c>
+      <c r="C14" t="n">
+        <v>0.03875202206385977</v>
+      </c>
+      <c r="D14" t="n">
+        <v>1285.142542309079</v>
+      </c>
+      <c r="E14" t="n">
+        <v>0.03757566950819195</v>
+      </c>
+      <c r="F14" t="n">
+        <v>2049.803926316772</v>
+      </c>
+      <c r="G14" t="n">
+        <v>1285.142592311579</v>
+      </c>
+      <c r="H14" t="n">
+        <v>5369.4965065584</v>
+      </c>
+      <c r="I14" t="n">
+        <v>1.050132323463516</v>
+      </c>
+      <c r="J14" t="n">
+        <v>37.14589851753538</v>
+      </c>
+      <c r="K14" t="n">
+        <v>0.458570113522252</v>
+      </c>
+      <c r="L14" t="n">
+        <v>2.100264646927031</v>
+      </c>
+      <c r="M14" t="inlineStr">
+        <is>
+          <t>Flagged Warnings:</t>
+        </is>
+      </c>
+      <c r="N14" t="n">
+        <v>1387.887922044903</v>
+      </c>
+      <c r="O14" t="n">
+        <v>0.009475667525246327</v>
+      </c>
+      <c r="P14" t="n">
+        <v>3062.457282870359</v>
+      </c>
+      <c r="Q14" t="n">
+        <v>1387.887872042403</v>
+      </c>
+      <c r="R14" t="n">
+        <v>7538.723397614501</v>
+      </c>
+      <c r="S14" t="n">
+        <v>1.129390794943371</v>
+      </c>
+      <c r="T14" t="n">
+        <v>0</v>
+      </c>
+      <c r="U14" t="n">
+        <v>17.14356988008451</v>
+      </c>
+      <c r="V14" t="n">
+        <v>0.0722365058919005</v>
+      </c>
+      <c r="W14" t="n">
+        <v>2.258781589886742</v>
+      </c>
+      <c r="X14" t="inlineStr">
+        <is>
+          <t>Flagged Warnings:</t>
+        </is>
+      </c>
+      <c r="Y14" t="n">
+        <v>1264.254774520237</v>
+      </c>
+      <c r="Z14" t="n">
+        <v>1376.021666144913</v>
+      </c>
+      <c r="AA14" t="n">
+        <v>3.127820278875336</v>
+      </c>
+      <c r="AB14" t="n">
+        <v>1409.086835471461</v>
+      </c>
+      <c r="AC14" t="n">
+        <v>608.8931026897881</v>
+      </c>
+      <c r="AD14" t="n">
+        <v>0.9081013922909871</v>
+      </c>
+      <c r="AE14" t="inlineStr"/>
+      <c r="AF14" t="inlineStr"/>
+      <c r="AG14" t="inlineStr"/>
+      <c r="AH14" t="inlineStr"/>
+      <c r="AI14" t="inlineStr"/>
+      <c r="AJ14" t="inlineStr"/>
+      <c r="AK14" t="inlineStr"/>
+      <c r="AL14" t="inlineStr"/>
+      <c r="AM14" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>